<commit_message>
final 8 layer stackup.
</commit_message>
<xml_diff>
--- a/projects/FMC_DAC/stackup.xlsx
+++ b/projects/FMC_DAC/stackup.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="8-layer" sheetId="1" r:id="rId1"/>
-    <sheet name="6-layer" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>Copper Layer</t>
   </si>
@@ -63,10 +62,7 @@
     <t>Calculated Z0</t>
   </si>
   <si>
-    <t>top route</t>
-  </si>
-  <si>
-    <t>bottom route</t>
+    <t>Grace GA-170LL</t>
   </si>
 </sst>
 </file>
@@ -403,15 +399,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="4" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
@@ -460,11 +457,14 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
       <c r="E3">
-        <v>4.3</v>
+        <v>4.7</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -491,8 +491,11 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
       <c r="E5">
-        <v>4.3</v>
+        <v>4.7</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -513,11 +516,14 @@
       <c r="C7" t="s">
         <v>2</v>
       </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
       <c r="E7">
-        <v>4.3</v>
+        <v>4.7</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -535,11 +541,14 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
       <c r="E9">
-        <v>4.3</v>
+        <v>4.7</v>
       </c>
       <c r="F9">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -557,11 +566,14 @@
       <c r="C11" t="s">
         <v>2</v>
       </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
       <c r="E11">
-        <v>4.3</v>
+        <v>4.7</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -579,8 +591,11 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
       <c r="E13">
-        <v>4.3</v>
+        <v>4.7</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -610,11 +625,14 @@
       <c r="C15" t="s">
         <v>2</v>
       </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
       <c r="E15">
-        <v>4.3</v>
+        <v>4.7</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -631,7 +649,7 @@
     <row r="23" spans="6:6">
       <c r="F23">
         <f>+SUM(F2:F16)</f>
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -640,204 +658,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2">
-        <v>0.5</v>
-      </c>
-      <c r="G2">
-        <v>50</v>
-      </c>
-      <c r="H2">
-        <v>6.6</v>
-      </c>
-      <c r="I2">
-        <v>50.47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>4.3</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>4.3</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>4.3</v>
-      </c>
-      <c r="F7">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>4.3</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>4.3</v>
-      </c>
-      <c r="F11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12">
-        <v>0.5</v>
-      </c>
-      <c r="G12">
-        <v>50</v>
-      </c>
-      <c r="H12">
-        <v>6.6</v>
-      </c>
-      <c r="I12">
-        <v>50.47</v>
-      </c>
-    </row>
-    <row r="19" spans="6:6">
-      <c r="F19">
-        <f>+SUM(F2:F12)</f>
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Stackup updated with recommendations from fab engineer.
</commit_message>
<xml_diff>
--- a/projects/FMC_DAC/stackup.xlsx
+++ b/projects/FMC_DAC/stackup.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="8-layer" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -400,7 +399,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -409,7 +408,7 @@
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
@@ -452,6 +451,12 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>88</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="C3" t="s">
@@ -481,10 +486,10 @@
         <v>50</v>
       </c>
       <c r="H4">
-        <v>6.6</v>
+        <v>5</v>
       </c>
       <c r="I4">
-        <v>50.47</v>
+        <v>49.9</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -615,10 +620,10 @@
         <v>50</v>
       </c>
       <c r="H14">
-        <v>6.6</v>
+        <v>5</v>
       </c>
       <c r="I14">
-        <v>50.47</v>
+        <v>49.9</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -644,6 +649,12 @@
       </c>
       <c r="F16">
         <v>0</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="6:6">
@@ -655,16 +666,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
hand routing the 6 layer stackup.
</commit_message>
<xml_diff>
--- a/projects/FMC_DAC/stackup.xlsx
+++ b/projects/FMC_DAC/stackup.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="8-layer" sheetId="1" r:id="rId1"/>
+    <sheet name="6-layer" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="16">
   <si>
     <t>Copper Layer</t>
   </si>
@@ -398,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -666,4 +667,211 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>4.7</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>4.7</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>4.7</v>
+      </c>
+      <c r="F7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>4.7</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>4.7</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6">
+      <c r="F19">
+        <f>+SUM(F2:F12)</f>
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>